<commit_message>
Change ATCA to ATCA2 in 01.R at Mesquite
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/data-wrangling-intermediate/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD09FA6D-D917-404E-AF38-AE8EBC865E73}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0150554C-3A48-4157-9226-311B011F93C8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>tc={A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}</author>
   </authors>
   <commentList>
-    <comment ref="E60" authorId="0" shapeId="0" xr:uid="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
+    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="174">
   <si>
     <t>Site</t>
   </si>
@@ -536,6 +536,30 @@
   </si>
   <si>
     <t>Bouteloua spp., SRER</t>
+  </si>
+  <si>
+    <t>AVRCD</t>
+  </si>
+  <si>
+    <t>AMIN3</t>
+  </si>
+  <si>
+    <t>AMMEI2</t>
+  </si>
+  <si>
+    <t>Amsinckia menziesii</t>
+  </si>
+  <si>
+    <t>LACA7</t>
+  </si>
+  <si>
+    <t>Lasthenia californica</t>
+  </si>
+  <si>
+    <t>PEPE26</t>
+  </si>
+  <si>
+    <t>Pectocarya penicillata</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1116,8 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>565784</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>24765</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -1508,7 +1532,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E60" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
+  <threadedComment ref="E63" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
     <text>USDA code is actually LILE29</text>
   </threadedComment>
 </ThreadedComments>
@@ -1516,11 +1540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C66056-BDB3-4C93-9739-661D41665B2E}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1578,13 +1602,13 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1607,7 +1631,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1639,16 +1663,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -3393,31 +3417,31 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G59" t="s">
         <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="I59" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>160</v>
@@ -3425,28 +3449,28 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
       </c>
       <c r="H60" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I60" t="s">
         <v>26</v>
@@ -3457,54 +3481,54 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
-      </c>
-      <c r="E61" t="s">
-        <v>127</v>
-      </c>
-      <c r="F61" t="s">
-        <v>128</v>
+        <v>172</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="G61" t="s">
         <v>6</v>
       </c>
       <c r="H61" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="I61" t="s">
         <v>26</v>
       </c>
-      <c r="J61" t="s">
-        <v>18</v>
+      <c r="J61" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
-      </c>
-      <c r="E62" t="s">
-        <v>130</v>
-      </c>
-      <c r="F62" t="s">
-        <v>131</v>
+        <v>163</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="G62" t="s">
         <v>6</v>
@@ -3515,8 +3539,8 @@
       <c r="I62" t="s">
         <v>17</v>
       </c>
-      <c r="J62" t="s">
-        <v>18</v>
+      <c r="J62" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -3530,25 +3554,25 @@
         <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>129</v>
-      </c>
-      <c r="E63" t="s">
-        <v>130</v>
-      </c>
-      <c r="F63" t="s">
-        <v>131</v>
+        <v>124</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="G63" t="s">
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="I63" t="s">
-        <v>17</v>
-      </c>
-      <c r="J63" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -3562,13 +3586,13 @@
         <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E64" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F64" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G64" t="s">
         <v>6</v>
@@ -3577,7 +3601,7 @@
         <v>16</v>
       </c>
       <c r="I64" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J64" t="s">
         <v>18</v>
@@ -3594,13 +3618,13 @@
         <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E65" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F65" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G65" t="s">
         <v>6</v>
@@ -3623,16 +3647,16 @@
         <v>123</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E66" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F66" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G66" t="s">
         <v>6</v>
@@ -3658,13 +3682,13 @@
         <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G67" t="s">
         <v>6</v>
@@ -3690,13 +3714,13 @@
         <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E68" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G68" t="s">
         <v>6</v>
@@ -3713,22 +3737,22 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
         <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D69" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F69" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G69" t="s">
         <v>6</v>
@@ -3737,7 +3761,7 @@
         <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J69" t="s">
         <v>18</v>
@@ -3745,22 +3769,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B70" t="s">
         <v>123</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D70" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E70" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F70" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G70" t="s">
         <v>6</v>
@@ -3777,22 +3801,22 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B71" t="s">
         <v>123</v>
       </c>
       <c r="C71" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E71" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F71" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G71" t="s">
         <v>6</v>
@@ -3815,16 +3839,16 @@
         <v>123</v>
       </c>
       <c r="C72" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D72" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F72" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G72" t="s">
         <v>6</v>
@@ -3833,7 +3857,7 @@
         <v>16</v>
       </c>
       <c r="I72" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J72" t="s">
         <v>18</v>
@@ -3850,13 +3874,13 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F73" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G73" t="s">
         <v>6</v>
@@ -3873,7 +3897,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B74" t="s">
         <v>123</v>
@@ -3885,10 +3909,10 @@
         <v>132</v>
       </c>
       <c r="E74" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F74" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G74" t="s">
         <v>6</v>
@@ -3905,22 +3929,22 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s">
         <v>123</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D75" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E75" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F75" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G75" t="s">
         <v>6</v>
@@ -3937,22 +3961,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B76" t="s">
         <v>123</v>
       </c>
       <c r="C76" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E76" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F76" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G76" t="s">
         <v>6</v>
@@ -3975,27 +3999,123 @@
         <v>123</v>
       </c>
       <c r="C77" t="s">
+        <v>55</v>
+      </c>
+      <c r="D77" t="s">
+        <v>132</v>
+      </c>
+      <c r="E77" t="s">
+        <v>151</v>
+      </c>
+      <c r="F77" t="s">
+        <v>152</v>
+      </c>
+      <c r="G77" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" t="s">
+        <v>135</v>
+      </c>
+      <c r="E78" t="s">
+        <v>153</v>
+      </c>
+      <c r="F78" t="s">
+        <v>154</v>
+      </c>
+      <c r="G78" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" t="s">
         <v>51</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D79" t="s">
+        <v>138</v>
+      </c>
+      <c r="E79" t="s">
+        <v>155</v>
+      </c>
+      <c r="F79" t="s">
+        <v>156</v>
+      </c>
+      <c r="G79" t="s">
+        <v>6</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" t="s">
+        <v>51</v>
+      </c>
+      <c r="D80" t="s">
         <v>157</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E80" t="s">
         <v>158</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F80" t="s">
         <v>159</v>
       </c>
-      <c r="G77" t="s">
-        <v>6</v>
-      </c>
-      <c r="H77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I77" t="s">
-        <v>17</v>
-      </c>
-      <c r="J77" t="s">
+      <c r="G80" t="s">
+        <v>6</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got through 03.1.R with Shriver (complete) data
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/data-wrangling-intermediate/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1910FAE6-7D0A-4CDE-8CA7-F7269F154365}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40AEC6CF-7E42-4A2D-A06A-850AAA07D1E1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="169">
   <si>
     <t>Site</t>
   </si>
@@ -82,15 +82,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>ATCA</t>
-  </si>
-  <si>
-    <t>ATCA.Mesquite</t>
-  </si>
-  <si>
-    <t>Unknown ATCA (but not Atriplex, a grass?), Mesquite</t>
-  </si>
-  <si>
     <t>Unkforb</t>
   </si>
   <si>
@@ -394,12 +385,6 @@
     <t>Utah</t>
   </si>
   <si>
-    <t>LILE</t>
-  </si>
-  <si>
-    <t>Leptosiphon lemmonii</t>
-  </si>
-  <si>
     <t>S-UNFO2</t>
   </si>
   <si>
@@ -542,9 +527,6 @@
   </si>
   <si>
     <t>Pectocarya penicillata</t>
-  </si>
-  <si>
-    <t>LILE29</t>
   </si>
 </sst>
 </file>
@@ -1101,13 +1083,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>565784</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>468629</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1212,10 +1194,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1515,11 +1493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C66056-BDB3-4C93-9739-661D41665B2E}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1577,13 +1555,13 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1606,7 +1584,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1638,16 +1616,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1656,7 +1634,7 @@
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1673,13 +1651,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1688,7 +1666,7 @@
         <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -1702,16 +1680,16 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1734,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1749,10 +1727,10 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -1760,31 +1738,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s">
         <v>18</v>
@@ -1792,22 +1770,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1824,13 +1802,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -1856,13 +1834,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
@@ -1888,10 +1866,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1920,22 +1898,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -1952,22 +1930,22 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -1984,22 +1962,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" t="s">
-        <v>54</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -2016,22 +1994,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -2048,13 +2026,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -2072,7 +2050,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
         <v>18</v>
@@ -2080,23 +2058,23 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>60</v>
       </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2082,7 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
@@ -2112,22 +2090,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -2144,22 +2122,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
         <v>62</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -2176,151 +2154,151 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" t="s">
-        <v>69</v>
-      </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
-        <v>69</v>
-      </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
       <c r="G24" t="s">
         <v>6</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>160</v>
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>72</v>
       </c>
-      <c r="F25" t="s">
-        <v>73</v>
-      </c>
       <c r="G25" t="s">
         <v>6</v>
       </c>
@@ -2328,7 +2306,7 @@
         <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J25" t="s">
         <v>18</v>
@@ -2336,22 +2314,22 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G26" t="s">
         <v>6</v>
@@ -2368,149 +2346,149 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
         <v>66</v>
       </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" t="s">
-        <v>16</v>
-      </c>
       <c r="I27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G28" t="s">
         <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G29" t="s">
         <v>6</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G30" t="s">
         <v>6</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" t="s">
         <v>79</v>
       </c>
       <c r="G31" t="s">
@@ -2520,30 +2498,30 @@
         <v>16</v>
       </c>
       <c r="I31" t="s">
-        <v>26</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>160</v>
+        <v>23</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G32" t="s">
         <v>6</v>
@@ -2552,7 +2530,7 @@
         <v>16</v>
       </c>
       <c r="I32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J32" t="s">
         <v>18</v>
@@ -2560,23 +2538,23 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>81</v>
       </c>
-      <c r="F33" t="s">
-        <v>82</v>
-      </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
@@ -2584,7 +2562,7 @@
         <v>16</v>
       </c>
       <c r="I33" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J33" t="s">
         <v>18</v>
@@ -2592,22 +2570,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
         <v>6</v>
@@ -2624,16 +2602,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
         <v>83</v>
@@ -2656,22 +2634,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G36" t="s">
         <v>6</v>
@@ -2688,22 +2666,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
         <v>85</v>
       </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>86</v>
-      </c>
-      <c r="F37" t="s">
-        <v>87</v>
       </c>
       <c r="G37" t="s">
         <v>6</v>
@@ -2720,22 +2698,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
         <v>85</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" t="s">
-        <v>88</v>
-      </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G38" t="s">
         <v>6</v>
@@ -2752,16 +2730,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E39" t="s">
         <v>88</v>
@@ -2784,22 +2762,22 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G40" t="s">
         <v>6</v>
@@ -2816,22 +2794,22 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
       </c>
       <c r="E41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" t="s">
         <v>91</v>
-      </c>
-      <c r="F41" t="s">
-        <v>92</v>
       </c>
       <c r="G41" t="s">
         <v>6</v>
@@ -2848,22 +2826,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" t="s">
         <v>90</v>
       </c>
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" t="s">
-        <v>93</v>
-      </c>
       <c r="F42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G42" t="s">
         <v>6</v>
@@ -2880,22 +2858,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
         <v>41</v>
       </c>
       <c r="E43" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" t="s">
         <v>93</v>
-      </c>
-      <c r="F43" t="s">
-        <v>94</v>
       </c>
       <c r="G43" t="s">
         <v>6</v>
@@ -2912,22 +2890,22 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G44" t="s">
         <v>6</v>
@@ -2944,10 +2922,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -2956,10 +2934,10 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" t="s">
         <v>95</v>
-      </c>
-      <c r="F45" t="s">
-        <v>96</v>
       </c>
       <c r="G45" t="s">
         <v>6</v>
@@ -2976,22 +2954,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F46" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G46" t="s">
         <v>6</v>
@@ -3008,21 +2986,21 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>98</v>
       </c>
       <c r="G47" t="s">
@@ -3034,29 +3012,29 @@
       <c r="I47" t="s">
         <v>17</v>
       </c>
-      <c r="J47" t="s">
-        <v>18</v>
+      <c r="J47" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
         <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
-      </c>
-      <c r="E48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="E48" t="s">
         <v>101</v>
       </c>
+      <c r="F48" t="s">
+        <v>102</v>
+      </c>
       <c r="G48" t="s">
         <v>6</v>
       </c>
@@ -3064,31 +3042,31 @@
         <v>16</v>
       </c>
       <c r="I48" t="s">
-        <v>17</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>160</v>
+        <v>23</v>
+      </c>
+      <c r="J48" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
       </c>
       <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" t="s">
         <v>103</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>104</v>
       </c>
-      <c r="F49" t="s">
-        <v>105</v>
-      </c>
       <c r="G49" t="s">
         <v>6</v>
       </c>
@@ -3096,7 +3074,7 @@
         <v>16</v>
       </c>
       <c r="I49" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J49" t="s">
         <v>18</v>
@@ -3104,22 +3082,22 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F50" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G50" t="s">
         <v>6</v>
@@ -3128,7 +3106,7 @@
         <v>16</v>
       </c>
       <c r="I50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J50" t="s">
         <v>18</v>
@@ -3136,23 +3114,23 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" t="s">
         <v>106</v>
       </c>
-      <c r="F51" t="s">
-        <v>107</v>
-      </c>
       <c r="G51" t="s">
         <v>6</v>
       </c>
@@ -3160,7 +3138,7 @@
         <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J51" t="s">
         <v>18</v>
@@ -3168,22 +3146,22 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E52" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F52" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G52" t="s">
         <v>6</v>
@@ -3200,23 +3178,23 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F53" t="s">
-        <v>109</v>
-      </c>
       <c r="G53" t="s">
         <v>6</v>
       </c>
@@ -3226,27 +3204,27 @@
       <c r="I53" t="s">
         <v>17</v>
       </c>
-      <c r="J53" t="s">
-        <v>18</v>
+      <c r="J53" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
         <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>99</v>
-      </c>
-      <c r="E54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" t="s">
         <v>110</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" t="s">
         <v>111</v>
       </c>
       <c r="G54" t="s">
@@ -3256,30 +3234,30 @@
         <v>16</v>
       </c>
       <c r="I54" t="s">
-        <v>17</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>160</v>
+        <v>31</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F55" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G55" t="s">
         <v>6</v>
@@ -3288,7 +3266,7 @@
         <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J55" t="s">
         <v>18</v>
@@ -3296,23 +3274,23 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" t="s">
         <v>112</v>
       </c>
-      <c r="B56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" t="s">
-        <v>51</v>
-      </c>
-      <c r="D56" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>113</v>
       </c>
-      <c r="F56" t="s">
-        <v>114</v>
-      </c>
       <c r="G56" t="s">
         <v>6</v>
       </c>
@@ -3320,7 +3298,7 @@
         <v>16</v>
       </c>
       <c r="I56" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="J56" t="s">
         <v>18</v>
@@ -3328,23 +3306,23 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
-      </c>
-      <c r="E57" t="s">
-        <v>115</v>
-      </c>
-      <c r="F57" t="s">
         <v>116</v>
       </c>
+      <c r="E57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="G57" t="s">
         <v>6</v>
       </c>
@@ -3354,156 +3332,156 @@
       <c r="I57" t="s">
         <v>17</v>
       </c>
-      <c r="J57" t="s">
-        <v>18</v>
+      <c r="J57" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D58" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="G58" t="s">
         <v>6</v>
       </c>
       <c r="H58" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="I58" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B59" t="s">
-        <v>118</v>
-      </c>
-      <c r="C59" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" t="s">
-        <v>167</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="G59" t="s">
         <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I59" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D60" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="I60" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="G61" t="s">
         <v>6</v>
       </c>
       <c r="H61" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I61" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>165</v>
+        <v>121</v>
+      </c>
+      <c r="E62" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" t="s">
+        <v>123</v>
       </c>
       <c r="G62" t="s">
         <v>6</v>
@@ -3512,63 +3490,63 @@
         <v>16</v>
       </c>
       <c r="I62" t="s">
-        <v>17</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>160</v>
+        <v>23</v>
+      </c>
+      <c r="J62" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D63" t="s">
         <v>124</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="E63" t="s">
         <v>125</v>
       </c>
+      <c r="F63" t="s">
+        <v>126</v>
+      </c>
       <c r="G63" t="s">
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I63" t="s">
-        <v>26</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>160</v>
+        <v>17</v>
+      </c>
+      <c r="J63" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D64" t="s">
+        <v>124</v>
+      </c>
+      <c r="E64" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" t="s">
         <v>126</v>
       </c>
-      <c r="E64" t="s">
-        <v>127</v>
-      </c>
-      <c r="F64" t="s">
-        <v>128</v>
-      </c>
       <c r="G64" t="s">
         <v>6</v>
       </c>
@@ -3576,7 +3554,7 @@
         <v>16</v>
       </c>
       <c r="I64" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J64" t="s">
         <v>18</v>
@@ -3584,22 +3562,22 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" t="s">
         <v>129</v>
-      </c>
-      <c r="E65" t="s">
-        <v>130</v>
-      </c>
-      <c r="F65" t="s">
-        <v>131</v>
       </c>
       <c r="G65" t="s">
         <v>6</v>
@@ -3616,22 +3594,22 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" t="s">
         <v>129</v>
-      </c>
-      <c r="E66" t="s">
-        <v>130</v>
-      </c>
-      <c r="F66" t="s">
-        <v>131</v>
       </c>
       <c r="G66" t="s">
         <v>6</v>
@@ -3648,22 +3626,22 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D67" t="s">
+        <v>130</v>
+      </c>
+      <c r="E67" t="s">
+        <v>131</v>
+      </c>
+      <c r="F67" t="s">
         <v>132</v>
-      </c>
-      <c r="E67" t="s">
-        <v>133</v>
-      </c>
-      <c r="F67" t="s">
-        <v>134</v>
       </c>
       <c r="G67" t="s">
         <v>6</v>
@@ -3680,22 +3658,22 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B68" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C68" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" t="s">
         <v>132</v>
-      </c>
-      <c r="E68" t="s">
-        <v>133</v>
-      </c>
-      <c r="F68" t="s">
-        <v>134</v>
       </c>
       <c r="G68" t="s">
         <v>6</v>
@@ -3712,22 +3690,22 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D69" t="s">
+        <v>133</v>
+      </c>
+      <c r="E69" t="s">
+        <v>134</v>
+      </c>
+      <c r="F69" t="s">
         <v>135</v>
-      </c>
-      <c r="E69" t="s">
-        <v>136</v>
-      </c>
-      <c r="F69" t="s">
-        <v>137</v>
       </c>
       <c r="G69" t="s">
         <v>6</v>
@@ -3744,22 +3722,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D70" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E70" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F70" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G70" t="s">
         <v>6</v>
@@ -3768,7 +3746,7 @@
         <v>16</v>
       </c>
       <c r="I70" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J70" t="s">
         <v>18</v>
@@ -3776,16 +3754,16 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E71" t="s">
         <v>139</v>
@@ -3808,23 +3786,23 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" t="s">
         <v>141</v>
       </c>
-      <c r="B72" t="s">
-        <v>123</v>
-      </c>
-      <c r="C72" t="s">
-        <v>55</v>
-      </c>
-      <c r="D72" t="s">
-        <v>126</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>142</v>
       </c>
-      <c r="F72" t="s">
-        <v>143</v>
-      </c>
       <c r="G72" t="s">
         <v>6</v>
       </c>
@@ -3832,7 +3810,7 @@
         <v>16</v>
       </c>
       <c r="I72" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J72" t="s">
         <v>18</v>
@@ -3840,22 +3818,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73" t="s">
         <v>141</v>
       </c>
-      <c r="B73" t="s">
-        <v>123</v>
-      </c>
-      <c r="C73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D73" t="s">
-        <v>129</v>
-      </c>
-      <c r="E73" t="s">
-        <v>144</v>
-      </c>
       <c r="F73" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G73" t="s">
         <v>6</v>
@@ -3872,22 +3850,22 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C74" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F74" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G74" t="s">
         <v>6</v>
@@ -3904,16 +3882,16 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B75" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D75" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E75" t="s">
         <v>146</v>
@@ -3936,16 +3914,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B76" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C76" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D76" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E76" t="s">
         <v>148</v>
@@ -3968,22 +3946,22 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" t="s">
+        <v>133</v>
+      </c>
+      <c r="E77" t="s">
         <v>150</v>
       </c>
-      <c r="B77" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77" t="s">
-        <v>55</v>
-      </c>
-      <c r="D77" t="s">
-        <v>132</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>151</v>
-      </c>
-      <c r="F77" t="s">
-        <v>152</v>
       </c>
       <c r="G77" t="s">
         <v>6</v>
@@ -4000,16 +3978,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D78" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="E78" t="s">
         <v>153</v>
@@ -4027,70 +4005,6 @@
         <v>17</v>
       </c>
       <c r="J78" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>150</v>
-      </c>
-      <c r="B79" t="s">
-        <v>123</v>
-      </c>
-      <c r="C79" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" t="s">
-        <v>138</v>
-      </c>
-      <c r="E79" t="s">
-        <v>155</v>
-      </c>
-      <c r="F79" t="s">
-        <v>156</v>
-      </c>
-      <c r="G79" t="s">
-        <v>6</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>17</v>
-      </c>
-      <c r="J79" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>150</v>
-      </c>
-      <c r="B80" t="s">
-        <v>123</v>
-      </c>
-      <c r="C80" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" t="s">
-        <v>157</v>
-      </c>
-      <c r="E80" t="s">
-        <v>158</v>
-      </c>
-      <c r="F80" t="s">
-        <v>159</v>
-      </c>
-      <c r="G80" t="s">
-        <v>6</v>
-      </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
-        <v>17</v>
-      </c>
-      <c r="J80" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>